<commit_message>
feat: add upload file and supabase
</commit_message>
<xml_diff>
--- a/docs/PLANTILLA.xlsx
+++ b/docs/PLANTILLA.xlsx
@@ -29,9 +29,6 @@
     <t>NombreCompleto</t>
   </si>
   <si>
-    <t>Alberto Romero Fulanito</t>
-  </si>
-  <si>
     <t>Comadre Petra Emilia</t>
   </si>
   <si>
@@ -152,10 +149,13 @@
     <t>LinkPdf</t>
   </si>
   <si>
-    <t>https://r1cordas.wordpress.com/wp-content/uploads/2017/06/manual-de-guitarra-ralph-denyer-en-espac3b1ol.pdf</t>
-  </si>
-  <si>
     <t>[["02/01/2025", "Otorgada","Médico Pana", "Observación 1"],["03/02/2025", "En espera","Médico", "Observación 2"]]</t>
+  </si>
+  <si>
+    <t>Alberto Fulanito</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1sp1StYshn1Fio4LQF9ORlnkTC0AQKnBI/view</t>
   </si>
 </sst>
 </file>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,148 +523,148 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
         <v>43</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: add redirect homepage
</commit_message>
<xml_diff>
--- a/docs/PLANTILLA.xlsx
+++ b/docs/PLANTILLA.xlsx
@@ -62,9 +62,6 @@
     <t>LugarOtorgamiento</t>
   </si>
   <si>
-    <t>Lugar 1</t>
-  </si>
-  <si>
     <t>Lugar 2</t>
   </si>
   <si>
@@ -89,18 +86,12 @@
     <t>ListadoDeTramitaciones</t>
   </si>
   <si>
-    <t>Salud 1</t>
-  </si>
-  <si>
     <t>Salud 2</t>
   </si>
   <si>
     <t>Salud 3</t>
   </si>
   <si>
-    <t>Medico 1</t>
-  </si>
-  <si>
     <t>Medico 2</t>
   </si>
   <si>
@@ -116,9 +107,6 @@
     <t>54631387-0</t>
   </si>
   <si>
-    <t>Social 1</t>
-  </si>
-  <si>
     <t>Social 2</t>
   </si>
   <si>
@@ -152,10 +140,22 @@
     <t>[["02/01/2025", "Otorgada","Médico Pana", "Observación 1"],["03/02/2025", "En espera","Médico", "Observación 2"]]</t>
   </si>
   <si>
-    <t>Alberto Fulanito</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/1sp1StYshn1Fio4LQF9ORlnkTC0AQKnBI/view</t>
+  </si>
+  <si>
+    <t>Jesús Lara</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Instituto Pedrito</t>
+  </si>
+  <si>
+    <t>Jose Ramirez</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -538,33 +538,33 @@
         <v>11</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -573,30 +573,30 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -608,33 +608,33 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
         <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -646,25 +646,25 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="I4" t="s">
-        <v>29</v>
-      </c>
       <c r="J4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>